<commit_message>
introduction of shear module, incorporation of style policies, flexure updates, beam module updates
</commit_message>
<xml_diff>
--- a/assets/run_2.xlsx
+++ b/assets/run_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://killa-my.sharepoint.com/personal/adnan_a_killadesign_com/Documents/github repositories/beam_scheduler/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{511469A0-B223-4FBF-9BBF-3E4C6BFA81C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{511469A0-B223-4FBF-9BBF-3E4C6BFA81C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5E5E2C-CA02-486A-9E93-88CA65D0E2C7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DAE23863-3E93-4A43-A0EF-08AC3AE6A99A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{DAE23863-3E93-4A43-A0EF-08AC3AE6A99A}"/>
   </bookViews>
   <sheets>
     <sheet name="Conc Bm Flx Env - ACI 318-19" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="130">
   <si>
     <t>TABLE:  Concrete Beam Flexure Envelope - ACI 318-19</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>ACI 318-19</t>
+  </si>
+  <si>
+    <t>O/S</t>
   </si>
 </sst>
 </file>
@@ -875,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AB371F-721B-4E36-899F-790388D9EB42}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O25" sqref="O25"/>
     </sheetView>
@@ -2563,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3FBA16-2B25-4D5F-A109-F7987CEE723E}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2727,7 +2730,7 @@
         <v>1877.96</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="K4">
         <v>28.311599999999999</v>

</xml_diff>

<commit_message>
finalised gui and main
</commit_message>
<xml_diff>
--- a/assets/run_2.xlsx
+++ b/assets/run_2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{511469A0-B223-4FBF-9BBF-3E4C6BFA81C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD5E5E2C-CA02-486A-9E93-88CA65D0E2C7}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{DAE23863-3E93-4A43-A0EF-08AC3AE6A99A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{DAE23863-3E93-4A43-A0EF-08AC3AE6A99A}"/>
   </bookViews>
   <sheets>
     <sheet name="Conc Bm Flx Env - ACI 318-19" sheetId="1" r:id="rId1"/>
@@ -2566,7 +2566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3FBA16-2B25-4D5F-A109-F7987CEE723E}">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -4825,9 +4825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEB6A1D-464E-49C6-BE8D-CCE253B9B721}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>